<commit_message>
Added Voice to Assetlist
</commit_message>
<xml_diff>
--- a/sketch/Sound Assetlist.xlsx
+++ b/sketch/Sound Assetlist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDFC9A2-B76F-4E23-A8D9-117A1DBE011F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7B2825-441A-452F-9E3E-37DB5EBA0176}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Summer" sheetId="6" r:id="rId7"/>
     <sheet name="Factory" sheetId="7" r:id="rId8"/>
     <sheet name="Interaction SFX" sheetId="11" r:id="rId9"/>
-    <sheet name="Music" sheetId="9" r:id="rId10"/>
+    <sheet name="Voice" sheetId="12" r:id="rId10"/>
+    <sheet name="Music" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="208">
   <si>
     <t>File Name</t>
   </si>
@@ -629,6 +630,30 @@
   </si>
   <si>
     <t>interaction_success</t>
+  </si>
+  <si>
+    <t>Voice words</t>
+  </si>
+  <si>
+    <t>should be very robotic</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Break</t>
   </si>
 </sst>
 </file>
@@ -683,7 +708,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,6 +841,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -844,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -885,6 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2189,6 +2221,120 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A08ADBF-0156-4855-95C9-C0D0EF140B64}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" style="5" customWidth="1"/>
+    <col min="4" max="5" width="15.77734375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A511E283-359F-4B23-A7FD-2B1984BC6E67}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -3494,8 +3640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D5EB9A-558E-45AE-867C-31B7DD80BC6E}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>